<commit_message>
Added "Sell at x-R" functionality.
</commit_message>
<xml_diff>
--- a/Inputs/DailyTradingPlan_DE.xlsx
+++ b/Inputs/DailyTradingPlan_DE.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\PycharmProjects\Momentum-Trading-Assistant\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\PycharmProjects\ibbot-python311\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BB92FC-C826-406D-9BFE-068CB70FF170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17BDF5DA-0751-4426-ACCC-CEDD4B811C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -31,279 +34,291 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
   <si>
     <t>Symbol</t>
   </si>
   <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Exchange</t>
+  </si>
+  <si>
+    <t>Primary Exchange</t>
+  </si>
+  <si>
+    <t>Entry price [$]</t>
+  </si>
+  <si>
+    <t>Stop price [$]</t>
+  </si>
+  <si>
+    <t>Quantity [#]</t>
+  </si>
+  <si>
+    <t>Buy limit price [$]</t>
+  </si>
+  <si>
+    <t>Profit taker price [$]</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>SMART</t>
+  </si>
+  <si>
+    <t>Security Type</t>
+  </si>
+  <si>
     <t>Company name</t>
   </si>
   <si>
-    <t>Security Type</t>
-  </si>
-  <si>
-    <t>Currency</t>
-  </si>
-  <si>
-    <t>Exchange</t>
-  </si>
-  <si>
-    <t>Primary Exchange</t>
-  </si>
-  <si>
-    <t>Entry price [$]</t>
-  </si>
-  <si>
-    <t>Stop price [$]</t>
-  </si>
-  <si>
-    <t>Quantity [#]</t>
-  </si>
-  <si>
-    <t>Buy limit price [$]</t>
-  </si>
-  <si>
-    <t>Profit taker price [$]</t>
+    <t>BID size</t>
+  </si>
+  <si>
+    <t>ASK size</t>
+  </si>
+  <si>
+    <t>Stop undercut</t>
+  </si>
+  <si>
+    <t>LAST price [$]</t>
+  </si>
+  <si>
+    <t>BID price [$]</t>
+  </si>
+  <si>
+    <t>ASK price [$]</t>
+  </si>
+  <si>
+    <t>CLOSE price [$]</t>
+  </si>
+  <si>
+    <t>Spread at execution [%]</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>parentOrderId</t>
+  </si>
+  <si>
+    <t>Crossed buy price</t>
+  </si>
+  <si>
+    <t>Stop undercut [time]</t>
+  </si>
+  <si>
+    <t>Crossed buy price [time]</t>
+  </si>
+  <si>
+    <t>2% above buy point</t>
+  </si>
+  <si>
+    <t>5% above buy point</t>
+  </si>
+  <si>
+    <t>Stock sold</t>
+  </si>
+  <si>
+    <t>Order filled</t>
+  </si>
+  <si>
+    <t>New OCA bracket</t>
+  </si>
+  <si>
+    <t>Order executed</t>
   </si>
   <si>
     <t>Open position</t>
   </si>
   <si>
+    <t>Stop timestamp</t>
+  </si>
+  <si>
+    <t>Open position bracket submitted</t>
+  </si>
+  <si>
+    <t>Last stop price</t>
+  </si>
+  <si>
+    <t>Order executed [time]</t>
+  </si>
+  <si>
+    <t>5% above buy point [time]</t>
+  </si>
+  <si>
+    <t>New OCA bracket [time]</t>
+  </si>
+  <si>
+    <t>Stock sold [time]</t>
+  </si>
+  <si>
+    <t>Invest limit reached</t>
+  </si>
+  <si>
+    <t>Max. daily loss reached</t>
+  </si>
+  <si>
+    <t>Invest limit reached [time]</t>
+  </si>
+  <si>
+    <t>Max. daily loss reached [time]</t>
+  </si>
+  <si>
     <t>Add and reduce</t>
   </si>
   <si>
+    <t>Add and reduce executed</t>
+  </si>
+  <si>
+    <t>profitOrderId</t>
+  </si>
+  <si>
+    <t>Profit order filled</t>
+  </si>
+  <si>
+    <t>stopOrderId</t>
+  </si>
+  <si>
+    <t>Stop order filled</t>
+  </si>
+  <si>
     <t>Sell on close</t>
   </si>
   <si>
+    <t>Sell bellow SMA [$]</t>
+  </si>
+  <si>
+    <t>Position below limit</t>
+  </si>
+  <si>
+    <t>sellOnCloseOrderId</t>
+  </si>
+  <si>
+    <t>SOC order filled</t>
+  </si>
+  <si>
+    <t>Spread above limit</t>
+  </si>
+  <si>
+    <t>Price above limit</t>
+  </si>
+  <si>
+    <t>Stock looped</t>
+  </si>
+  <si>
+    <t>Open position updated</t>
+  </si>
+  <si>
+    <t>Open position updated [time]</t>
+  </si>
+  <si>
+    <t>New position updated</t>
+  </si>
+  <si>
+    <t>New position updated [time]</t>
+  </si>
+  <si>
+    <t>New position added</t>
+  </si>
+  <si>
+    <t>New position added [time]</t>
+  </si>
+  <si>
+    <t>HIGH price [$]</t>
+  </si>
+  <si>
+    <t>LOW price [$]</t>
+  </si>
+  <si>
+    <t>Bad close rule</t>
+  </si>
+  <si>
+    <t>Bad close rule [time]</t>
+  </si>
+  <si>
+    <t>MAX_STOCK_SPREAD</t>
+  </si>
+  <si>
+    <t>SELL_HALF_REVERSAL_RULE</t>
+  </si>
+  <si>
+    <t>SELL_FULL_REVERSAL_RULE</t>
+  </si>
+  <si>
+    <t>MAX_ALLOWED_DAILY_PNL_LOSS</t>
+  </si>
+  <si>
+    <t>MIN_POSITION_SIZE</t>
+  </si>
+  <si>
+    <t>Bad close checked</t>
+  </si>
+  <si>
+    <t>liquidHours</t>
+  </si>
+  <si>
+    <t>timeZoneId</t>
+  </si>
+  <si>
+    <t>local opening time</t>
+  </si>
+  <si>
+    <t>local closing time</t>
+  </si>
+  <si>
+    <t>STK</t>
+  </si>
+  <si>
+    <t>BTC</t>
+  </si>
+  <si>
+    <t>CRYPTO</t>
+  </si>
+  <si>
+    <t>PAXOS</t>
+  </si>
+  <si>
     <t>Stop low of day</t>
   </si>
   <si>
-    <t>Sell bellow SMA [$]</t>
-  </si>
-  <si>
-    <t>Stop undercut [time]</t>
-  </si>
-  <si>
-    <t>Stop undercut</t>
-  </si>
-  <si>
-    <t>Crossed buy price [time]</t>
-  </si>
-  <si>
-    <t>Crossed buy price</t>
-  </si>
-  <si>
-    <t>Order executed [time]</t>
-  </si>
-  <si>
-    <t>Order executed</t>
-  </si>
-  <si>
-    <t>parentOrderId</t>
-  </si>
-  <si>
-    <t>Order filled</t>
-  </si>
-  <si>
-    <t>profitOrderId</t>
-  </si>
-  <si>
-    <t>Profit order filled</t>
-  </si>
-  <si>
-    <t>stopOrderId</t>
-  </si>
-  <si>
-    <t>Stop order filled</t>
-  </si>
-  <si>
-    <t>sellOnCloseOrderId</t>
-  </si>
-  <si>
-    <t>SOC order filled</t>
-  </si>
-  <si>
-    <t>Spread at execution [%]</t>
-  </si>
-  <si>
-    <t>2% above buy point</t>
-  </si>
-  <si>
-    <t>New OCA bracket [time]</t>
-  </si>
-  <si>
-    <t>New OCA bracket</t>
-  </si>
-  <si>
-    <t>5% above buy point [time]</t>
-  </si>
-  <si>
-    <t>5% above buy point</t>
-  </si>
-  <si>
-    <t>Bad close rule [time]</t>
-  </si>
-  <si>
-    <t>Bad close rule</t>
-  </si>
-  <si>
-    <t>Stock sold [time]</t>
-  </si>
-  <si>
-    <t>Stock sold</t>
-  </si>
-  <si>
-    <t>Spread above limit</t>
-  </si>
-  <si>
-    <t>Price above limit</t>
-  </si>
-  <si>
-    <t>Stock looped</t>
-  </si>
-  <si>
-    <t>Open position bracket submitted</t>
-  </si>
-  <si>
-    <t>Add and reduce executed</t>
-  </si>
-  <si>
-    <t>Open position updated</t>
-  </si>
-  <si>
-    <t>Open position updated [time]</t>
-  </si>
-  <si>
-    <t>New position updated</t>
-  </si>
-  <si>
-    <t>New position updated [time]</t>
-  </si>
-  <si>
-    <t>New position added</t>
-  </si>
-  <si>
-    <t>New position added [time]</t>
-  </si>
-  <si>
-    <t>Stop timestamp</t>
-  </si>
-  <si>
-    <t>Last stop price</t>
-  </si>
-  <si>
-    <t>Invest limit reached [time]</t>
-  </si>
-  <si>
-    <t>Invest limit reached</t>
-  </si>
-  <si>
-    <t>Position below limit</t>
-  </si>
-  <si>
-    <t>Max. daily loss reached [time]</t>
-  </si>
-  <si>
-    <t>Max. daily loss reached</t>
-  </si>
-  <si>
-    <t>LAST price [$]</t>
-  </si>
-  <si>
-    <t>BID price [$]</t>
-  </si>
-  <si>
-    <t>ASK price [$]</t>
-  </si>
-  <si>
-    <t>BID size</t>
-  </si>
-  <si>
-    <t>ASK size</t>
-  </si>
-  <si>
-    <t>HIGH price [$]</t>
-  </si>
-  <si>
-    <t>LOW price [$]</t>
-  </si>
-  <si>
-    <t>CLOSE price [$]</t>
-  </si>
-  <si>
-    <t>Volume</t>
-  </si>
-  <si>
-    <t>MAX_STOCK_SPREAD</t>
-  </si>
-  <si>
-    <t>SELL_HALF_REVERSAL_RULE</t>
-  </si>
-  <si>
-    <t>SELL_FULL_REVERSAL_RULE</t>
-  </si>
-  <si>
     <t>BAD_CLOSE_RULE</t>
   </si>
   <si>
-    <t>MAX_ALLOWED_DAILY_PNL_LOSS</t>
-  </si>
-  <si>
-    <t>MIN_POSITION_SIZE</t>
-  </si>
-  <si>
-    <t>Bad close checked</t>
-  </si>
-  <si>
-    <t>liquidHours</t>
-  </si>
-  <si>
-    <t>timeZoneId</t>
-  </si>
-  <si>
-    <t>local opening time</t>
-  </si>
-  <si>
-    <t>local closing time</t>
-  </si>
-  <si>
-    <t>BTC</t>
-  </si>
-  <si>
-    <t>CRYPTO</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>SMART</t>
-  </si>
-  <si>
-    <t>PAXOS</t>
-  </si>
-  <si>
-    <t>STK</t>
+    <t>Sell negative on day 1</t>
+  </si>
+  <si>
+    <t>Negative close checked</t>
+  </si>
+  <si>
+    <t>marketOrderId</t>
+  </si>
+  <si>
+    <t>Market order filled</t>
+  </si>
+  <si>
+    <t>Market sell price [$]</t>
+  </si>
+  <si>
+    <t>Profit at x-R</t>
+  </si>
+  <si>
+    <t>x-R profits [time]</t>
+  </si>
+  <si>
+    <t>x-R profits</t>
+  </si>
+  <si>
+    <t>RHM</t>
   </si>
   <si>
     <t>EUR</t>
   </si>
   <si>
     <t>IBIS</t>
-  </si>
-  <si>
-    <t>Sell negative on day 1</t>
-  </si>
-  <si>
-    <t>Negative close checked</t>
-  </si>
-  <si>
-    <t>RHM</t>
-  </si>
-  <si>
-    <t>TKA</t>
-  </si>
-  <si>
-    <t>HAG</t>
   </si>
 </sst>
 </file>
@@ -356,7 +371,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="List Panel Header" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="List Panel Header" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -670,10 +685,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:CC290"/>
+  <dimension ref="A1:CI290"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -692,331 +707,353 @@
     <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.33203125" customWidth="1"/>
     <col min="14" max="16" width="14.77734375" customWidth="1"/>
-    <col min="17" max="17" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17.109375" customWidth="1"/>
-    <col min="32" max="32" width="15.6640625" customWidth="1"/>
-    <col min="33" max="33" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.88671875" customWidth="1"/>
+    <col min="20" max="20" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.109375" customWidth="1"/>
+    <col min="33" max="33" width="15.6640625" customWidth="1"/>
+    <col min="34" max="34" width="13.77734375" customWidth="1"/>
+    <col min="35" max="36" width="17.88671875" customWidth="1"/>
+    <col min="37" max="37" width="21.77734375" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="19" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.44140625" customWidth="1"/>
-    <col min="41" max="41" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="15.88671875" customWidth="1"/>
-    <col min="45" max="45" width="13" customWidth="1"/>
-    <col min="46" max="46" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="23.33203125" customWidth="1"/>
-    <col min="49" max="49" width="27.21875" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="52" max="53" width="26.5546875" customWidth="1"/>
-    <col min="54" max="54" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="23" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="17.88671875" customWidth="1"/>
-    <col min="59" max="59" width="27" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="24.77734375" customWidth="1"/>
-    <col min="61" max="61" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="66" max="67" width="12.33203125" customWidth="1"/>
-    <col min="68" max="68" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="29.5546875" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="16" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="13.21875" customWidth="1"/>
-    <col min="79" max="79" width="11.21875" customWidth="1"/>
-    <col min="80" max="80" width="16" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="19" bestFit="1" customWidth="1"/>
+    <col min="44" max="45" width="17.44140625" customWidth="1"/>
+    <col min="46" max="46" width="16" customWidth="1"/>
+    <col min="47" max="47" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="15.88671875" customWidth="1"/>
+    <col min="51" max="51" width="13" customWidth="1"/>
+    <col min="52" max="52" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="23.33203125" customWidth="1"/>
+    <col min="55" max="55" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="58" max="59" width="26.5546875" customWidth="1"/>
+    <col min="60" max="60" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="23" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="17.88671875" customWidth="1"/>
+    <col min="65" max="65" width="27" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="24.77734375" customWidth="1"/>
+    <col min="67" max="67" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="72" max="73" width="12.33203125" customWidth="1"/>
+    <col min="74" max="74" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="16" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="13.21875" customWidth="1"/>
+    <col min="85" max="85" width="11.21875" customWidth="1"/>
+    <col min="86" max="86" width="16" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:87" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="O1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" t="s">
+        <v>84</v>
+      </c>
+      <c r="S1" t="s">
+        <v>89</v>
+      </c>
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" t="s">
+        <v>15</v>
+      </c>
+      <c r="V1" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" t="s">
+        <v>23</v>
+      </c>
+      <c r="X1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>34</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>45</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>35</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>42</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>40</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>43</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>41</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>17</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>18</v>
+      </c>
+      <c r="BR1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="BS1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
-        <v>86</v>
-      </c>
-      <c r="R1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" t="s">
-        <v>18</v>
-      </c>
-      <c r="V1" t="s">
+      <c r="BT1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BV1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" t="s">
-        <v>20</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="BW1" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>49</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>50</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>54</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>55</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>56</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>57</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>58</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>59</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BL1" t="s">
-        <v>61</v>
-      </c>
-      <c r="BM1" t="s">
-        <v>62</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>63</v>
-      </c>
-      <c r="BO1" t="s">
-        <v>64</v>
-      </c>
-      <c r="BP1" t="s">
-        <v>65</v>
-      </c>
-      <c r="BQ1" t="s">
-        <v>66</v>
-      </c>
-      <c r="BR1" t="s">
-        <v>67</v>
-      </c>
-      <c r="BS1" t="s">
+      <c r="BX1" t="s">
         <v>68</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BY1" t="s">
         <v>69</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BZ1" t="s">
         <v>70</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="CA1" t="s">
+        <v>83</v>
+      </c>
+      <c r="CB1" t="s">
         <v>71</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="CC1" t="s">
         <v>72</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="CD1" t="s">
         <v>73</v>
       </c>
-      <c r="BY1" t="s">
-        <v>87</v>
-      </c>
-      <c r="BZ1" t="s">
+      <c r="CE1" t="s">
+        <v>85</v>
+      </c>
+      <c r="CF1" t="s">
         <v>74</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CG1" t="s">
         <v>75</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CH1" t="s">
         <v>76</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CI1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:87" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E2" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
         <v>81</v>
-      </c>
-      <c r="G2" t="s">
-        <v>82</v>
       </c>
       <c r="H2" s="1">
         <v>9</v>
@@ -1034,218 +1071,129 @@
         <v>11.25</v>
       </c>
     </row>
-    <row r="3" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:87" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E3" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>81</v>
+        <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="H3" s="1">
-        <v>1700</v>
+        <v>1773</v>
       </c>
       <c r="I3" s="1">
-        <v>1650</v>
+        <v>1750</v>
       </c>
       <c r="J3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>1720</v>
+        <v>1790.73</v>
       </c>
       <c r="L3">
-        <v>2500</v>
+        <v>2038.95</v>
       </c>
       <c r="M3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:81" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" s="1">
-        <v>10</v>
-      </c>
-      <c r="I4" s="1">
-        <v>9</v>
-      </c>
-      <c r="J4" s="2">
+      <c r="O3" t="b">
         <v>1</v>
       </c>
-      <c r="K4">
-        <v>11</v>
-      </c>
-      <c r="L4">
-        <v>13</v>
-      </c>
-      <c r="M4" t="b">
+      <c r="P3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:81" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G5" t="s">
-        <v>85</v>
-      </c>
-      <c r="H5" s="1">
-        <v>96</v>
-      </c>
-      <c r="I5" s="1">
-        <v>95</v>
-      </c>
-      <c r="J5" s="2">
+      <c r="Q3">
+        <v>64.5</v>
+      </c>
+      <c r="R3" t="b">
         <v>1</v>
       </c>
-      <c r="K5">
-        <v>125</v>
-      </c>
-      <c r="L5">
-        <v>125</v>
-      </c>
-      <c r="M5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:81" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G6" t="s">
-        <v>85</v>
-      </c>
-      <c r="H6" s="1">
-        <v>96</v>
-      </c>
-      <c r="I6" s="1">
-        <v>95</v>
-      </c>
-      <c r="J6" s="2">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <v>125</v>
-      </c>
-      <c r="L6">
-        <v>125</v>
-      </c>
-      <c r="M6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:81" x14ac:dyDescent="0.3">
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+    </row>
+    <row r="4" spans="1:87" x14ac:dyDescent="0.3">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:87" x14ac:dyDescent="0.3">
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:87" x14ac:dyDescent="0.3">
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:87" x14ac:dyDescent="0.3">
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:81" x14ac:dyDescent="0.3">
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+    <row r="8" spans="1:87" x14ac:dyDescent="0.3">
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:87" x14ac:dyDescent="0.3">
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:87" x14ac:dyDescent="0.3">
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:87" x14ac:dyDescent="0.3">
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:87" x14ac:dyDescent="0.3">
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:87" x14ac:dyDescent="0.3">
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:87" x14ac:dyDescent="0.3">
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:87" x14ac:dyDescent="0.3">
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:87" x14ac:dyDescent="0.3">
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="2"/>
@@ -2622,6 +2570,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>